<commit_message>
add benders for endogenous
</commit_message>
<xml_diff>
--- a/generator/overnightcost.xlsx
+++ b/generator/overnightcost.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/canli/euler/work/GETP/generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5486CF88-3A47-3442-BD02-5A62F5A39061}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E426BF-DF5F-6845-B448-BF158E45DA55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38600" yWindow="2200" windowWidth="38200" windowHeight="19400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42560" yWindow="3040" windowWidth="38200" windowHeight="19400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Year</t>
   </si>
@@ -69,15 +69,25 @@
   </si>
   <si>
     <t>ratio from ES-4</t>
+  </si>
+  <si>
+    <t>old data from NREL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -92,7 +102,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -100,14 +110,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -401,7 +428,7 @@
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,7 +460,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -467,7 +494,7 @@
         <v>1355000</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>20</v>
       </c>
@@ -502,7 +529,7 @@
         <v>1252000</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -520,6 +547,85 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3">
+        <v>7595435.0059829392</v>
+      </c>
+      <c r="C7" s="3">
+        <v>4403066.8345398102</v>
+      </c>
+      <c r="D7" s="3">
+        <v>8336982.970066403</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2197663.7787233214</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1056219.7820617117</v>
+      </c>
+      <c r="G7" s="3">
+        <v>903008.18696589826</v>
+      </c>
+      <c r="H7" s="4">
+        <v>6368644.7459658151</v>
+      </c>
+      <c r="I7" s="3">
+        <v>1942417.1494312561</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1805373.2913492424</v>
+      </c>
+      <c r="K7">
+        <f>(J7-J2)/J7</f>
+        <v>0.2494626975525138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>20</v>
+      </c>
+      <c r="B8" s="3">
+        <v>6688134.3088378394</v>
+      </c>
+      <c r="C8" s="3">
+        <v>4020859.7434782488</v>
+      </c>
+      <c r="D8" s="3">
+        <v>3671272.8565971311</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1885564.3582574772</v>
+      </c>
+      <c r="F8" s="3">
+        <v>972045.09040297195</v>
+      </c>
+      <c r="G8" s="3">
+        <v>825931.58690454136</v>
+      </c>
+      <c r="H8" s="4">
+        <v>5962845.7648886573</v>
+      </c>
+      <c r="I8" s="3">
+        <v>999618.32806695125</v>
+      </c>
+      <c r="J8" s="3">
+        <v>1611214.5406524658</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I10">
+        <f>(I7-I2)/I7</f>
+        <v>0.11347570190872477</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>